<commit_message>
updated bphc, drc, gbsc with resolve
</commit_message>
<xml_diff>
--- a/InputData/elec/BPHC/BAU Pumped Hydro Cap.xlsx
+++ b/InputData/elec/BPHC/BAU Pumped Hydro Cap.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Documents\EPS_Models by Region\RMI\California\CA-eps\InputData\elec\BPHC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{419564CA-6B76-4D0B-8A34-00E98C3F9651}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35E1AB1F-CE42-4F09-99A0-34F2D683C4ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8110" yWindow="260" windowWidth="16940" windowHeight="13590" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5490" yWindow="400" windowWidth="18840" windowHeight="13240" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -614,7 +614,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -624,6 +624,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEAC6FE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -640,7 +646,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -660,6 +666,7 @@
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -28928,15 +28935,17 @@
   </sheetPr>
   <dimension ref="B2:AJ224"/>
   <sheetViews>
-    <sheetView topLeftCell="N18" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23:AJ23"/>
+    <sheetView topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="M65" sqref="M65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="2" width="8.6640625" style="8"/>
     <col min="3" max="3" width="22.5" style="8" customWidth="1"/>
-    <col min="4" max="16384" width="8.6640625" style="8"/>
+    <col min="4" max="5" width="8.6640625" style="8"/>
+    <col min="6" max="12" width="0" style="8" hidden="1" customWidth="1"/>
+    <col min="13" max="16384" width="8.6640625" style="8"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:36" x14ac:dyDescent="0.35">
@@ -33493,7 +33502,7 @@
       <c r="L65" s="8">
         <v>0</v>
       </c>
-      <c r="M65" s="8">
+      <c r="M65" s="13">
         <v>1898.5</v>
       </c>
       <c r="N65" s="8">
@@ -45817,37 +45826,48 @@
         <v>42</v>
       </c>
       <c r="C2" s="8">
-        <v>0</v>
+        <f>'CEC_RESOLVE_38MMT PSP'!M65</f>
+        <v>1898.5</v>
       </c>
       <c r="D2" s="8">
-        <v>0</v>
+        <f>'CEC_RESOLVE_38MMT PSP'!N65</f>
+        <v>1898.5</v>
       </c>
       <c r="E2" s="8">
-        <v>0</v>
+        <f>'CEC_RESOLVE_38MMT PSP'!O65</f>
+        <v>1898.5</v>
       </c>
       <c r="F2" s="8">
-        <v>0</v>
+        <f>'CEC_RESOLVE_38MMT PSP'!P65</f>
+        <v>1898.5</v>
       </c>
       <c r="G2" s="8">
-        <v>196</v>
+        <f>'CEC_RESOLVE_38MMT PSP'!Q65</f>
+        <v>2094.5</v>
       </c>
       <c r="H2" s="8">
-        <v>1000</v>
+        <f>G2</f>
+        <v>2094.5</v>
       </c>
       <c r="I2" s="8">
-        <v>1000.28</v>
+        <f>'CEC_RESOLVE_38MMT PSP'!S65</f>
+        <v>2898.5</v>
       </c>
       <c r="J2" s="8">
-        <v>1000.28</v>
+        <f>I2</f>
+        <v>2898.5</v>
       </c>
       <c r="K2" s="8">
-        <v>1000.28</v>
+        <f>'CEC_RESOLVE_38MMT PSP'!U65</f>
+        <v>2898.7799999999997</v>
       </c>
       <c r="L2" s="8">
-        <v>1000.28</v>
+        <f>K2</f>
+        <v>2898.7799999999997</v>
       </c>
       <c r="M2" s="8">
-        <v>1000.28</v>
+        <f>'CEC_RESOLVE_38MMT PSP'!W65</f>
+        <v>2898.7799999999997</v>
       </c>
     </row>
     <row r="4" spans="2:34" x14ac:dyDescent="0.3">
@@ -45959,116 +45979,120 @@
         <v>0</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <f>C2</f>
+        <v>1898.5</v>
       </c>
       <c r="G5">
-        <v>0</v>
+        <f t="shared" ref="G5:I5" si="0">D2</f>
+        <v>1898.5</v>
       </c>
       <c r="H5">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>1898.5</v>
       </c>
       <c r="I5">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>1898.5</v>
       </c>
       <c r="J5">
         <f>_xlfn.FORECAST.LINEAR(J$4,$G$2:$H$2,$G$1:$H$1)</f>
-        <v>196</v>
+        <v>2094.5</v>
       </c>
       <c r="K5">
-        <f t="shared" ref="K5:M5" si="0">_xlfn.FORECAST.LINEAR(K$4,$G$2:$H$2,$G$1:$H$1)</f>
-        <v>598</v>
+        <f t="shared" ref="K5:L5" si="1">_xlfn.FORECAST.LINEAR(K$4,$G$2:$H$2,$G$1:$H$1)</f>
+        <v>2094.5</v>
       </c>
       <c r="L5">
-        <f t="shared" si="0"/>
-        <v>1000</v>
+        <f t="shared" si="1"/>
+        <v>2094.5</v>
       </c>
       <c r="M5">
         <f>_xlfn.FORECAST.LINEAR(M$4,$H$2:$I$2,$H$1:$I$1)</f>
-        <v>1000.14</v>
+        <v>2496.5</v>
       </c>
       <c r="N5">
-        <f t="shared" ref="N5:P5" si="1">_xlfn.FORECAST.LINEAR(N$4,$H$2:$I$2,$H$1:$I$1)</f>
-        <v>1000.28</v>
+        <f t="shared" ref="N5" si="2">_xlfn.FORECAST.LINEAR(N$4,$H$2:$I$2,$H$1:$I$1)</f>
+        <v>2898.5</v>
       </c>
       <c r="O5">
         <f>$N$5</f>
-        <v>1000.28</v>
+        <v>2898.5</v>
       </c>
       <c r="P5">
-        <f t="shared" ref="P5:AH5" si="2">$N$5</f>
-        <v>1000.28</v>
+        <f t="shared" ref="P5:AH5" si="3">$N$5</f>
+        <v>2898.5</v>
       </c>
       <c r="Q5">
-        <f t="shared" si="2"/>
-        <v>1000.28</v>
+        <f t="shared" si="3"/>
+        <v>2898.5</v>
       </c>
       <c r="R5">
-        <f t="shared" si="2"/>
-        <v>1000.28</v>
+        <f t="shared" si="3"/>
+        <v>2898.5</v>
       </c>
       <c r="S5">
-        <f t="shared" si="2"/>
-        <v>1000.28</v>
+        <f t="shared" si="3"/>
+        <v>2898.5</v>
       </c>
       <c r="T5">
-        <f t="shared" si="2"/>
-        <v>1000.28</v>
+        <f t="shared" si="3"/>
+        <v>2898.5</v>
       </c>
       <c r="U5">
-        <f t="shared" si="2"/>
-        <v>1000.28</v>
+        <f t="shared" si="3"/>
+        <v>2898.5</v>
       </c>
       <c r="V5">
-        <f t="shared" si="2"/>
-        <v>1000.28</v>
+        <f t="shared" si="3"/>
+        <v>2898.5</v>
       </c>
       <c r="W5">
-        <f t="shared" si="2"/>
-        <v>1000.28</v>
+        <f t="shared" si="3"/>
+        <v>2898.5</v>
       </c>
       <c r="X5">
-        <f t="shared" si="2"/>
-        <v>1000.28</v>
+        <f t="shared" si="3"/>
+        <v>2898.5</v>
       </c>
       <c r="Y5">
-        <f t="shared" si="2"/>
-        <v>1000.28</v>
+        <f t="shared" si="3"/>
+        <v>2898.5</v>
       </c>
       <c r="Z5">
-        <f t="shared" si="2"/>
-        <v>1000.28</v>
+        <f t="shared" si="3"/>
+        <v>2898.5</v>
       </c>
       <c r="AA5">
-        <f t="shared" si="2"/>
-        <v>1000.28</v>
+        <f t="shared" si="3"/>
+        <v>2898.5</v>
       </c>
       <c r="AB5">
-        <f t="shared" si="2"/>
-        <v>1000.28</v>
+        <f t="shared" si="3"/>
+        <v>2898.5</v>
       </c>
       <c r="AC5">
-        <f t="shared" si="2"/>
-        <v>1000.28</v>
+        <f t="shared" si="3"/>
+        <v>2898.5</v>
       </c>
       <c r="AD5">
-        <f t="shared" si="2"/>
-        <v>1000.28</v>
+        <f t="shared" si="3"/>
+        <v>2898.5</v>
       </c>
       <c r="AE5">
-        <f t="shared" si="2"/>
-        <v>1000.28</v>
+        <f t="shared" si="3"/>
+        <v>2898.5</v>
       </c>
       <c r="AF5">
-        <f t="shared" si="2"/>
-        <v>1000.28</v>
+        <f t="shared" si="3"/>
+        <v>2898.5</v>
       </c>
       <c r="AG5">
-        <f t="shared" si="2"/>
-        <v>1000.28</v>
+        <f t="shared" si="3"/>
+        <v>2898.5</v>
       </c>
       <c r="AH5">
-        <f t="shared" si="2"/>
-        <v>1000.28</v>
+        <f t="shared" si="3"/>
+        <v>2898.5</v>
       </c>
     </row>
   </sheetData>
@@ -46212,119 +46236,119 @@
       </c>
       <c r="E2" s="10">
         <f>'CA BPHC'!F5</f>
-        <v>0</v>
+        <v>1898.5</v>
       </c>
       <c r="F2" s="10">
         <f>'CA BPHC'!G5</f>
-        <v>0</v>
+        <v>1898.5</v>
       </c>
       <c r="G2" s="10">
         <f>'CA BPHC'!H5</f>
-        <v>0</v>
+        <v>1898.5</v>
       </c>
       <c r="H2" s="10">
         <f>'CA BPHC'!I5</f>
-        <v>0</v>
+        <v>1898.5</v>
       </c>
       <c r="I2" s="10">
         <f>'CA BPHC'!J5</f>
-        <v>196</v>
+        <v>2094.5</v>
       </c>
       <c r="J2" s="10">
         <f>'CA BPHC'!K5</f>
-        <v>598</v>
+        <v>2094.5</v>
       </c>
       <c r="K2" s="10">
         <f>'CA BPHC'!L5</f>
-        <v>1000</v>
+        <v>2094.5</v>
       </c>
       <c r="L2" s="10">
         <f>'CA BPHC'!M5</f>
-        <v>1000.14</v>
+        <v>2496.5</v>
       </c>
       <c r="M2" s="10">
         <f>'CA BPHC'!N5</f>
-        <v>1000.28</v>
+        <v>2898.5</v>
       </c>
       <c r="N2" s="10">
         <f>'CA BPHC'!O5</f>
-        <v>1000.28</v>
+        <v>2898.5</v>
       </c>
       <c r="O2" s="10">
         <f>'CA BPHC'!P5</f>
-        <v>1000.28</v>
+        <v>2898.5</v>
       </c>
       <c r="P2" s="10">
         <f>'CA BPHC'!Q5</f>
-        <v>1000.28</v>
+        <v>2898.5</v>
       </c>
       <c r="Q2" s="10">
         <f>'CA BPHC'!R5</f>
-        <v>1000.28</v>
+        <v>2898.5</v>
       </c>
       <c r="R2" s="10">
         <f>'CA BPHC'!S5</f>
-        <v>1000.28</v>
+        <v>2898.5</v>
       </c>
       <c r="S2" s="10">
         <f>'CA BPHC'!T5</f>
-        <v>1000.28</v>
+        <v>2898.5</v>
       </c>
       <c r="T2" s="10">
         <f>'CA BPHC'!U5</f>
-        <v>1000.28</v>
+        <v>2898.5</v>
       </c>
       <c r="U2" s="10">
         <f>'CA BPHC'!V5</f>
-        <v>1000.28</v>
+        <v>2898.5</v>
       </c>
       <c r="V2" s="10">
         <f>'CA BPHC'!W5</f>
-        <v>1000.28</v>
+        <v>2898.5</v>
       </c>
       <c r="W2" s="10">
         <f>'CA BPHC'!X5</f>
-        <v>1000.28</v>
+        <v>2898.5</v>
       </c>
       <c r="X2" s="10">
         <f>'CA BPHC'!Y5</f>
-        <v>1000.28</v>
+        <v>2898.5</v>
       </c>
       <c r="Y2" s="10">
         <f>'CA BPHC'!Z5</f>
-        <v>1000.28</v>
+        <v>2898.5</v>
       </c>
       <c r="Z2" s="10">
         <f>'CA BPHC'!AA5</f>
-        <v>1000.28</v>
+        <v>2898.5</v>
       </c>
       <c r="AA2" s="10">
         <f>'CA BPHC'!AB5</f>
-        <v>1000.28</v>
+        <v>2898.5</v>
       </c>
       <c r="AB2" s="10">
         <f>'CA BPHC'!AC5</f>
-        <v>1000.28</v>
+        <v>2898.5</v>
       </c>
       <c r="AC2" s="10">
         <f>'CA BPHC'!AD5</f>
-        <v>1000.28</v>
+        <v>2898.5</v>
       </c>
       <c r="AD2" s="10">
         <f>'CA BPHC'!AE5</f>
-        <v>1000.28</v>
+        <v>2898.5</v>
       </c>
       <c r="AE2" s="10">
         <f>'CA BPHC'!AF5</f>
-        <v>1000.28</v>
+        <v>2898.5</v>
       </c>
       <c r="AF2" s="10">
         <f>'CA BPHC'!AG5</f>
-        <v>1000.28</v>
+        <v>2898.5</v>
       </c>
       <c r="AG2" s="10">
         <f>'CA BPHC'!AH5</f>
-        <v>1000.28</v>
+        <v>2898.5</v>
       </c>
     </row>
     <row r="3" spans="1:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">

</xml_diff>